<commit_message>
Visual results done (MS SSIM)
</commit_message>
<xml_diff>
--- a/Phase2TestResults.xlsx
+++ b/Phase2TestResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Thesis\RSM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4012EBBE-4243-45C9-AB02-F94E31B1854B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7893B914-F8D8-43D1-8CE7-661B4FAB8CCC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{33346624-15BD-4DAD-9F42-9F5FEEA33BF9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Framerate</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>SNC Deferred Interpolated</t>
+  </si>
+  <si>
+    <t>MSSSIM Direct Illum Only</t>
+  </si>
+  <si>
+    <t>MSSSIM Deferred Interpolated</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>(artifacts on walls!)</t>
   </si>
 </sst>
 </file>
@@ -448,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1843DC63-62B7-4213-ACA5-0FDB45433A82}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,6 +989,56 @@
         <v>47.9</v>
       </c>
     </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18">
+        <v>0.77039813999999995</v>
+      </c>
+      <c r="G18">
+        <v>0.89640003000000001</v>
+      </c>
+      <c r="J18">
+        <v>0.82853776000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <v>0.78431229999999996</v>
+      </c>
+      <c r="G19">
+        <v>0.89153223999999998</v>
+      </c>
+      <c r="J19">
+        <v>0.83168489999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20">
+        <f>0.7843123-0.77039814</f>
+        <v>1.3914160000000009E-2</v>
+      </c>
+      <c r="G20">
+        <f>0.89153224-0.89640003</f>
+        <v>-4.8677900000000385E-3</v>
+      </c>
+      <c r="J20">
+        <f>0.8316849-0.82853776</f>
+        <v>3.1471399999999372E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Phase 2 Test Results
</commit_message>
<xml_diff>
--- a/Phase2TestResults.xlsx
+++ b/Phase2TestResults.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Thesis\RSM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF98722-4994-40D2-B62E-6CEB41FABC06}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D24C13-471C-4CB4-A358-A2759561E2F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{33346624-15BD-4DAD-9F42-9F5FEEA33BF9}"/>
   </bookViews>
@@ -21,12 +21,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="42">
   <si>
     <t>Framerate</t>
   </si>
@@ -128,6 +133,30 @@
   </si>
   <si>
     <t>Lucy</t>
+  </si>
+  <si>
+    <t>MSSSIM Accelerated</t>
+  </si>
+  <si>
+    <t>MSSSIM Forward</t>
+  </si>
+  <si>
+    <t>MSSSIM Deferred</t>
+  </si>
+  <si>
+    <t>No RSM</t>
+  </si>
+  <si>
+    <t>Forward</t>
+  </si>
+  <si>
+    <t>Deferred</t>
+  </si>
+  <si>
+    <t>Accelerated</t>
+  </si>
+  <si>
+    <t>Accelerated Deferred</t>
   </si>
 </sst>
 </file>
@@ -273,7 +302,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naive</c:v>
+                  <c:v>Forward</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -338,7 +367,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Naive</c:v>
+                  <c:v>Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -403,7 +432,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Interpolated</c:v>
+                  <c:v>Accelerated Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -460,7 +489,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -803,7 +831,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naive</c:v>
+                  <c:v>Forward</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -868,7 +896,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Naive</c:v>
+                  <c:v>Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -933,7 +961,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Interpolated</c:v>
+                  <c:v>Accelerated Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1332,7 +1360,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naive</c:v>
+                  <c:v>Forward</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1397,7 +1425,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Naive</c:v>
+                  <c:v>Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1462,7 +1490,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Interpolated</c:v>
+                  <c:v>Accelerated Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1861,7 +1889,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naive</c:v>
+                  <c:v>Forward</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1926,7 +1954,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Naive</c:v>
+                  <c:v>Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1991,7 +2019,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Interpolated</c:v>
+                  <c:v>Accelerated Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2390,7 +2418,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naive</c:v>
+                  <c:v>Forward</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2455,7 +2483,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Naive</c:v>
+                  <c:v>Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2520,7 +2548,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Interpolated</c:v>
+                  <c:v>Accelerated Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3907,6 +3935,983 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>MS-SSIM</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>SNC</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data Vis'!$E$106</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SNC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Vis'!$D$107:$D$110</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>No RSM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Forward</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Deferred</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Accelerated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Vis'!$E$107:$E$110</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.82853776000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83185319999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83172363000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83168489999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3505-4F37-A470-1F7B209F213E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="569833096"/>
+        <c:axId val="569834408"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="569833096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="569834408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="569834408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="569833096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>MS-SSIM - </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Lucy</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data Vis'!$G$106</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lucy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Vis'!$F$107:$F$110</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>No RSM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Forward</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Deferred</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Accelerated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Vis'!$G$107:$G$110</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.89640003000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89201909999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89136462999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89153223999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-84C2-47B1-A87A-CED062171213}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="704514424"/>
+        <c:axId val="704516392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="704514424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="704516392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="704516392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="704514424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>MS-SSIM - </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sponza</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data Vis'!$I$106</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sponza</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Vis'!$H$107:$H$110</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>No RSM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Forward</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Deferred</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Accelerated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Vis'!$I$107:$I$110</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.59985440000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.57229169999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57292419999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.57067279999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F86F-4260-9D27-5EB7110724B4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="704461616"/>
+        <c:axId val="704462600"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="704461616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="704462600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="704462600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="704461616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -3992,7 +4997,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naive</c:v>
+                  <c:v>Forward</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4057,7 +5062,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Naive</c:v>
+                  <c:v>Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4122,7 +5127,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Interpolated</c:v>
+                  <c:v>Accelerated Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4179,7 +5184,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4532,7 +5536,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naive</c:v>
+                  <c:v>Forward</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4597,7 +5601,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Naive</c:v>
+                  <c:v>Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4662,7 +5666,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Interpolated</c:v>
+                  <c:v>Accelerated Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5071,7 +6075,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naive</c:v>
+                  <c:v>Forward</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5136,7 +6140,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Naive</c:v>
+                  <c:v>Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5201,7 +6205,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Interpolated</c:v>
+                  <c:v>Accelerated Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5610,7 +6614,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naive</c:v>
+                  <c:v>Forward</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5675,7 +6679,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Naive</c:v>
+                  <c:v>Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5740,7 +6744,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Interpolated</c:v>
+                  <c:v>Accelerated Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6149,7 +7153,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naive</c:v>
+                  <c:v>Forward</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6214,7 +7218,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Naive</c:v>
+                  <c:v>Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6279,7 +7283,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Interpolated</c:v>
+                  <c:v>Accelerated Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6683,7 +7687,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naive</c:v>
+                  <c:v>Forward</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6748,7 +7752,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Naive</c:v>
+                  <c:v>Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6813,7 +7817,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Interpolated</c:v>
+                  <c:v>Accelerated Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7217,7 +8221,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naive</c:v>
+                  <c:v>Forward</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7282,7 +8286,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Naive</c:v>
+                  <c:v>Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7347,7 +8351,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Interpolated</c:v>
+                  <c:v>Accelerated Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7751,7 +8755,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Naive</c:v>
+                  <c:v>Forward</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7816,7 +8820,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Naive</c:v>
+                  <c:v>Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7881,7 +8885,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Deferred Interpolated</c:v>
+                  <c:v>Accelerated Deferred</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8454,6 +9458,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
@@ -11769,6 +12893,1515 @@
 </file>
 
 <file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -16837,6 +19470,114 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1000125</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="18" name="Chart 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D492C37D-841E-42C9-BDC8-9DDCCED6BEDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="19" name="Chart 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3BC866D-2AF5-4559-9551-DD6407FE08F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="20" name="Chart 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4506D1A7-D546-42C7-9D22-56629A0BB607}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -17137,10 +19878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3418115D-07C6-4736-9BB0-119CCFDC6B05}">
-  <dimension ref="A1:O87"/>
+  <dimension ref="A1:O110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U87" sqref="U87"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85:A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17186,7 +19927,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>59.7</v>
@@ -17198,7 +19939,7 @@
         <v>23.6</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="G2">
         <v>96.556955969482487</v>
@@ -17210,7 +19951,7 @@
         <v>97.390820656763111</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="M2">
         <v>24.79538635336618</v>
@@ -17224,7 +19965,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>48</v>
@@ -17236,7 +19977,7 @@
         <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="G3">
         <v>93.570213190573497</v>
@@ -17248,7 +19989,7 @@
         <v>93.209779311175041</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="M3">
         <v>23.029800222732092</v>
@@ -17262,7 +20003,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <v>55.4</v>
@@ -17274,7 +20015,7 @@
         <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G4">
         <v>93.615388786601926</v>
@@ -17286,7 +20027,7 @@
         <v>93.6813759254986</v>
       </c>
       <c r="L4" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="M4">
         <v>16.920084609367876</v>
@@ -17329,7 +20070,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B23">
         <v>35.816423399329238</v>
@@ -17367,7 +20108,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B24">
         <v>28.118862404066604</v>
@@ -17405,7 +20146,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B25">
         <v>20.991094019300373</v>
@@ -17472,7 +20213,7 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B44">
         <v>4.8743697004951472E-2</v>
@@ -17484,7 +20225,7 @@
         <v>1.6025886819450157</v>
       </c>
       <c r="F44" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="G44">
         <v>2274.5018070408692</v>
@@ -17496,7 +20237,7 @@
         <v>2061.3365334271862</v>
       </c>
       <c r="L44" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="M44">
         <v>279.862881798324</v>
@@ -17510,7 +20251,7 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B45">
         <v>3.7405384774434842E-2</v>
@@ -17522,7 +20263,7 @@
         <v>2.8477531911602183</v>
       </c>
       <c r="F45" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="G45">
         <v>1196.6350371651836</v>
@@ -17534,7 +20275,7 @@
         <v>843.1131840196922</v>
       </c>
       <c r="L45" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="M45">
         <v>121.00262940418574</v>
@@ -17548,7 +20289,7 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B46">
         <v>4.5539336240565491E-2</v>
@@ -17560,7 +20301,7 @@
         <v>3.2614043254046088</v>
       </c>
       <c r="F46" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G46">
         <v>493.35078192852012</v>
@@ -17572,7 +20313,7 @@
         <v>319.26076604990141</v>
       </c>
       <c r="L46" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="M46">
         <v>60.419789992844159</v>
@@ -17621,7 +20362,7 @@
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B65">
         <v>34.168468134887831</v>
@@ -17633,7 +20374,7 @@
         <v>44.537466962538254</v>
       </c>
       <c r="F65" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="G65">
         <v>111.5367851951768</v>
@@ -17645,7 +20386,7 @@
         <v>100.49610913643617</v>
       </c>
       <c r="L65" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="M65">
         <f>9082048836.63163/1024/1024</f>
@@ -17662,7 +20403,7 @@
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B66">
         <v>28.345655767186518</v>
@@ -17674,7 +20415,7 @@
         <v>44.636307579341945</v>
       </c>
       <c r="F66" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="G66">
         <v>64.545322653084781</v>
@@ -17686,7 +20427,7 @@
         <v>41.75420215034552</v>
       </c>
       <c r="L66" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="M66">
         <f>6670303216.74295/1024/1024</f>
@@ -17703,7 +20444,7 @@
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B67">
         <v>28.358274667067832</v>
@@ -17715,7 +20456,7 @@
         <v>44.636092964043328</v>
       </c>
       <c r="F67" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G67">
         <v>27.712908287812432</v>
@@ -17727,7 +20468,7 @@
         <v>14.827992374560587</v>
       </c>
       <c r="L67" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="M67">
         <f>2815398467.58313/1024/1024</f>
@@ -17773,7 +20514,7 @@
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B85">
         <f>8986016605.85647/1024/1024</f>
@@ -17788,7 +20529,7 @@
         <v>2161.8846513745116</v>
       </c>
       <c r="F85" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="G85">
         <f>277500111.46725/1024/1024</f>
@@ -17803,7 +20544,7 @@
         <v>83.298736502050403</v>
       </c>
       <c r="L85" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="M85">
         <v>3.5454874706408899</v>
@@ -17817,7 +20558,7 @@
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B86">
         <f>6552403703.48549/1024/1024</f>
@@ -17832,7 +20573,7 @@
         <v>2331.3544666546918</v>
       </c>
       <c r="F86" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="G86">
         <f>977837376.55302/1024/1024</f>
@@ -17847,7 +20588,7 @@
         <v>663.66363163775441</v>
       </c>
       <c r="L86" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="M86">
         <v>3.8274087921920836</v>
@@ -17861,7 +20602,7 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B87">
         <f>2694536720.9111/1024/1024</f>
@@ -17876,7 +20617,7 @@
         <v>2415.2664818550875</v>
       </c>
       <c r="F87" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G87">
         <f>796767022.242981/1024/1024</f>
@@ -17891,7 +20632,7 @@
         <v>601.37713981550314</v>
       </c>
       <c r="L87" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="M87">
         <v>3.9782409251121909</v>
@@ -17901,6 +20642,109 @@
       </c>
       <c r="O87">
         <v>8.4379063381291495</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E106" t="s">
+        <v>32</v>
+      </c>
+      <c r="G106" t="s">
+        <v>33</v>
+      </c>
+      <c r="I106" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>24</v>
+      </c>
+      <c r="D107" t="s">
+        <v>37</v>
+      </c>
+      <c r="E107">
+        <v>0.82853776000000001</v>
+      </c>
+      <c r="F107" t="s">
+        <v>37</v>
+      </c>
+      <c r="G107">
+        <v>0.89640003000000001</v>
+      </c>
+      <c r="H107" t="s">
+        <v>37</v>
+      </c>
+      <c r="I107">
+        <v>0.59985440000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>35</v>
+      </c>
+      <c r="D108" t="s">
+        <v>38</v>
+      </c>
+      <c r="E108">
+        <v>0.83185319999999996</v>
+      </c>
+      <c r="F108" t="s">
+        <v>38</v>
+      </c>
+      <c r="G108">
+        <v>0.89201909999999995</v>
+      </c>
+      <c r="H108" t="s">
+        <v>38</v>
+      </c>
+      <c r="I108">
+        <v>0.57229169999999996</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>36</v>
+      </c>
+      <c r="D109" t="s">
+        <v>39</v>
+      </c>
+      <c r="E109">
+        <v>0.83172363000000005</v>
+      </c>
+      <c r="F109" t="s">
+        <v>39</v>
+      </c>
+      <c r="G109">
+        <v>0.89136462999999999</v>
+      </c>
+      <c r="H109" t="s">
+        <v>39</v>
+      </c>
+      <c r="I109">
+        <v>0.57292419999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>34</v>
+      </c>
+      <c r="D110" t="s">
+        <v>40</v>
+      </c>
+      <c r="E110">
+        <v>0.83168489999999995</v>
+      </c>
+      <c r="F110" t="s">
+        <v>40</v>
+      </c>
+      <c r="G110">
+        <v>0.89153223999999998</v>
+      </c>
+      <c r="H110" t="s">
+        <v>40</v>
+      </c>
+      <c r="I110">
+        <v>0.57067279999999998</v>
       </c>
     </row>
   </sheetData>
@@ -17914,7 +20758,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A21" sqref="A18:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>